<commit_message>
cum in my mouth
</commit_message>
<xml_diff>
--- a/power_tree.xlsx
+++ b/power_tree.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Flore\OneDrive\Desktop\uni\session7\APP1\S7_PCB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69EF0266-A3B6-47CB-A9D1-7DA70C5ADBAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF9B9C03-B647-48A1-AC2B-013830312BBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -6165,8 +6165,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA2BDD99-5DF5-42E2-9FB8-4E21BAF0F6C9}">
   <dimension ref="A1:H38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F39" sqref="F39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6858,11 +6858,11 @@
     </row>
     <row r="36" spans="2:7" x14ac:dyDescent="0.25">
       <c r="F36" s="34">
-        <v>0.21</v>
+        <v>1</v>
       </c>
       <c r="G36" s="34">
         <f>F36*39.37</f>
-        <v>8.2676999999999996</v>
+        <v>39.369999999999997</v>
       </c>
     </row>
     <row r="37" spans="2:7" x14ac:dyDescent="0.25">
@@ -6875,11 +6875,11 @@
     </row>
     <row r="38" spans="2:7" x14ac:dyDescent="0.25">
       <c r="F38" s="34">
-        <v>17.716000000000001</v>
+        <v>1</v>
       </c>
       <c r="G38" s="34">
         <f>F38*0.0254</f>
-        <v>0.44998640000000001</v>
+        <v>2.5399999999999999E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>